<commit_message>
correção de lsim com AxBu -- ok
</commit_message>
<xml_diff>
--- a/plots/lsim.xlsx
+++ b/plots/lsim.xlsx
@@ -1252,11 +1252,11 @@
   </sheetPr>
   <dimension ref="A1:C202"/>
   <sheetViews>
-    <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="true" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A98" colorId="64" zoomScale="110" zoomScaleNormal="110" zoomScalePageLayoutView="100" workbookViewId="0">
-      <selection pane="topLeft" activeCell="A98" activeCellId="0" sqref="A:A"/>
+    <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="true" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="110" zoomScaleNormal="110" zoomScalePageLayoutView="100" workbookViewId="0">
+      <selection pane="topLeft" activeCell="C1" activeCellId="0" sqref="A:C"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="11.6875" defaultRowHeight="12.8" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
+  <sheetFormatPr defaultColWidth="11.72265625" defaultRowHeight="12.8" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
   <cols>
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="1024" min="1007" style="0" width="11.52"/>
   </cols>

</xml_diff>